<commit_message>
further updates paper 26112021
</commit_message>
<xml_diff>
--- a/data/TablesZhangetal2017_09_16_EN_21.xlsx
+++ b/data/TablesZhangetal2017_09_16_EN_21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rver4657\Dropbox (Sydney Uni)\Research\Forest_and_water\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BA5179-2A0D-4BD4-B6E0-52975E442E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC28E506-801B-4A5F-9CCD-86DA70F42EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="4" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{B1C3C98C-7119-441C-AC65-FC55BF675211}"/>
   </bookViews>
   <sheets>
     <sheet name="Zhang et al. (2017) &gt;1000km2" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5078" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5078" uniqueCount="901">
   <si>
     <t>Watershed #</t>
   </si>
@@ -2821,6 +2821,12 @@
   <si>
     <t xml:space="preserve">Aproximate loction defined by Roche's map in Amazon Region in French Guyana. Is is Amazon region? WV: This is not for the whole Amazon, but just for some small paired watershed studies in French Guyana, it is also unclear how they defined the change in forest and change in flow. Data should be removed from the analysis.
 </t>
+  </si>
+  <si>
+    <t>Abstract Baker 1984 says %Q  +157%, cound not find 599.1. The 599% is based on entry in Stednick et al 1996.  https://doi.org/10.1029/WR022i001p00067 and https://doi.org/10.1029/WR020i011p01639 Correct citation missing Baker, Jr., M.B., 1984. Changes in streamflow in an herbicide treated pinyon-juniper watershed in Arizona.
+Water Resour. Res., 20: 1639-1642.
+Baker, Jr., M.B., 1986. Effects of ponderosa pine treatments on water yield in Arizona. Water Resour. Res.,
+22: 67-73. CORRECTED the DELTA Qf to 157% based on Baker 1984 in csv</t>
   </si>
 </sst>
 </file>
@@ -7038,10 +7044,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C628113C-78B0-4B5D-8B46-887DA17257C6}">
   <dimension ref="A1:S257"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="10.199999999999999"/>
@@ -7505,7 +7511,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="153">
+    <row r="9" spans="1:19" ht="163.19999999999999">
       <c r="A9" s="29">
         <v>76</v>
       </c>
@@ -7550,7 +7556,7 @@
         <v>11</v>
       </c>
       <c r="P9" s="63" t="s">
-        <v>690</v>
+        <v>900</v>
       </c>
       <c r="Q9" s="64">
         <v>1958</v>
@@ -36752,7 +36758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B205A1BE-4CBB-47D7-9BF7-1F7EE06D6B2C}">
   <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>

</xml_diff>